<commit_message>
Añadiendo herramientas de lectura de excel
</commit_message>
<xml_diff>
--- a/src/test/resources/data/SalidaGarantiasDatos.xlsx
+++ b/src/test/resources/data/SalidaGarantiasDatos.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Repos\Pruebas Pipeline\prueba-ci-cd-dev\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE602ED-CD6C-4449-AEEF-CB9344EA0AD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BEE881C-9E17-4EAA-A29E-2A1B0A9AE270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{077DF315-AA34-4EED-86E6-A0454E45C536}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>TipoBusqueda</t>
   </si>
@@ -72,12 +72,46 @@
   </si>
   <si>
     <t>motivo2</t>
+  </si>
+  <si>
+    <t>estado</t>
+  </si>
+  <si>
+    <t>tipobusqueda3</t>
+  </si>
+  <si>
+    <t>tipobusqueda4</t>
+  </si>
+  <si>
+    <t>numeroDocumento3</t>
+  </si>
+  <si>
+    <t>garantia3</t>
+  </si>
+  <si>
+    <t>motivo3</t>
+  </si>
+  <si>
+    <t>numeroDocumento4</t>
+  </si>
+  <si>
+    <t>garantia4</t>
+  </si>
+  <si>
+    <t>motivo4</t>
+  </si>
+  <si>
+    <t>Creado</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -430,19 +464,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D64DE776-25B6-4517-B4B9-753890CBF249}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -455,8 +489,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -469,8 +506,11 @@
       <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -482,6 +522,43 @@
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>